<commit_message>
Minor part list and ID list fixes
</commit_message>
<xml_diff>
--- a/BOM/Unified Part List.xlsx
+++ b/BOM/Unified Part List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8392BA0-0F35-4488-AC3B-EFCFA2EA60E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658FE920-CA2B-47A7-BC8E-81EC1DD6E29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6EB0A7B6-C6D7-4759-8B58-841D5EFF92F5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2290" uniqueCount="1158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2297" uniqueCount="1161">
   <si>
     <t>ID</t>
   </si>
@@ -3406,9 +3406,6 @@
     <t>For heat shrink and butt splices</t>
   </si>
   <si>
-    <t>9 in 1 Folding Hex Key Set Metric Aluminum Allen Wrench Multi-Purposes Hex Key Tool Non-Slip for Construction Home Decoration - Walmart.com</t>
-  </si>
-  <si>
     <t>https://www.walmart.com/ip/Equate-91-Isopropyl-Alcohol-Antiseptic-32-fl-oz/276040459</t>
   </si>
   <si>
@@ -3509,6 +3506,18 @@
   </si>
   <si>
     <t>0.5lb to start; have heard mixed reviews of this supplier via Amazon</t>
+  </si>
+  <si>
+    <t>https://www.walmart.com/ip/9-in-1-Folding-Hex-Key-Set-Metric-Aluminum-Allen-Wrench-Multi-Purposes-Hex-Key-Tool-Non-Slip-for-Construction-Home-Decoration/723992410</t>
+  </si>
+  <si>
+    <t>UN014</t>
+  </si>
+  <si>
+    <t>Tape Measure, Metric</t>
+  </si>
+  <si>
+    <t>https://www.walmart.com/ip/Deli-Measuring-Tape-Measure-25-Ft-Metric-Imperial-Measurement-Tape-Retractable-Self-Lock/884432846</t>
   </si>
 </sst>
 </file>
@@ -3610,8 +3619,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}" name="Table13" displayName="Table13" ref="A1:J312" totalsRowShown="0">
-  <autoFilter ref="A1:J312" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}" name="Table13" displayName="Table13" ref="A1:J313" totalsRowShown="0">
+  <autoFilter ref="A1:J313" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J310">
     <sortCondition ref="A1:A310"/>
   </sortState>
@@ -3928,10 +3937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D318B5EB-87D8-4D97-AE82-574AF33D7DA4}">
-  <dimension ref="A1:J312"/>
+  <dimension ref="A1:J313"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
+      <selection activeCell="J313" sqref="J313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3987,7 +3996,7 @@
         <v>695</v>
       </c>
       <c r="C2" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="D2" t="s">
         <v>405</v>
@@ -4006,7 +4015,7 @@
       </c>
       <c r="I2" s="5"/>
       <c r="J2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -4068,59 +4077,59 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="B5" t="s">
         <v>695</v>
       </c>
       <c r="C5" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="D5" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5" t="s">
+        <v>1151</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>1152</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>1153</v>
-      </c>
       <c r="H5" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="B6" t="s">
         <v>695</v>
       </c>
       <c r="C6" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="D6" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>1154</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>1155</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -4371,7 +4380,7 @@
       </c>
       <c r="I15" s="5"/>
       <c r="J15" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -4401,7 +4410,7 @@
       </c>
       <c r="I16" s="5"/>
       <c r="J16" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -4454,7 +4463,7 @@
         <v>6</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="H18" t="s">
         <v>57</v>
@@ -4957,14 +4966,14 @@
         <v>6</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="H35" t="s">
         <v>57</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -5057,7 +5066,7 @@
       </c>
       <c r="I39" s="5"/>
       <c r="J39" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -8128,7 +8137,7 @@
         <v>6</v>
       </c>
       <c r="G159" s="3" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="H159" t="s">
         <v>57</v>
@@ -8674,13 +8683,13 @@
         <v>6</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="H180" t="s">
         <v>47</v>
       </c>
       <c r="I180" s="5" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="J180" t="s">
         <v>76</v>
@@ -8793,7 +8802,7 @@
         <v>89</v>
       </c>
       <c r="C185" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="D185" t="s">
         <v>404</v>
@@ -8819,7 +8828,7 @@
         <v>89</v>
       </c>
       <c r="C186" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="D186" t="s">
         <v>404</v>
@@ -8845,7 +8854,7 @@
         <v>89</v>
       </c>
       <c r="C187" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="D187" t="s">
         <v>404</v>
@@ -9243,13 +9252,13 @@
         <v>128</v>
       </c>
       <c r="G202" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="H202" t="s">
         <v>32</v>
       </c>
       <c r="I202" s="5" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="J202" t="s">
         <v>401</v>
@@ -9272,13 +9281,13 @@
         <v>128</v>
       </c>
       <c r="G203" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="H203" t="s">
         <v>32</v>
       </c>
       <c r="I203" s="5" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="J203" t="s">
         <v>401</v>
@@ -10058,7 +10067,7 @@
         <v>197</v>
       </c>
       <c r="H234" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="I234" s="5"/>
       <c r="J234" t="s">
@@ -10082,7 +10091,7 @@
         <v>197</v>
       </c>
       <c r="H235" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="I235" s="5"/>
       <c r="J235" t="s">
@@ -10106,7 +10115,7 @@
         <v>197</v>
       </c>
       <c r="H236" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="I236" s="5"/>
       <c r="J236" t="s">
@@ -10130,7 +10139,7 @@
         <v>197</v>
       </c>
       <c r="H237" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="I237" s="5"/>
       <c r="J237" t="s">
@@ -10154,7 +10163,7 @@
         <v>197</v>
       </c>
       <c r="H238" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="I238" s="5"/>
       <c r="J238" t="s">
@@ -10178,7 +10187,7 @@
         <v>197</v>
       </c>
       <c r="H239" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="I239" s="5"/>
       <c r="J239" t="s">
@@ -10202,7 +10211,7 @@
         <v>197</v>
       </c>
       <c r="H240" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="I240" s="5"/>
       <c r="J240" t="s">
@@ -10226,7 +10235,7 @@
         <v>197</v>
       </c>
       <c r="H241" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="I241" s="5"/>
       <c r="J241" t="s">
@@ -10250,7 +10259,7 @@
         <v>197</v>
       </c>
       <c r="H242" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="I242" s="5"/>
       <c r="J242" t="s">
@@ -10274,7 +10283,7 @@
         <v>197</v>
       </c>
       <c r="H243" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="I243" s="5"/>
       <c r="J243" t="s">
@@ -10417,7 +10426,7 @@
         <v>6</v>
       </c>
       <c r="G249" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="H249" t="s">
         <v>57</v>
@@ -11688,7 +11697,7 @@
         <v>1114</v>
       </c>
       <c r="G296" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="H296" t="s">
         <v>57</v>
@@ -11772,7 +11781,7 @@
         <v>6</v>
       </c>
       <c r="G299" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="H299" t="s">
         <v>57</v>
@@ -11802,7 +11811,7 @@
         <v>6</v>
       </c>
       <c r="G300" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="H300" t="s">
         <v>57</v>
@@ -12034,8 +12043,8 @@
       <c r="F308" t="s">
         <v>1114</v>
       </c>
-      <c r="G308" s="1" t="s">
-        <v>1123</v>
+      <c r="G308" t="s">
+        <v>1157</v>
       </c>
       <c r="H308" t="s">
         <v>57</v>
@@ -12154,7 +12163,7 @@
         <v>6</v>
       </c>
       <c r="G312" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="H312" t="s">
         <v>57</v>
@@ -12163,6 +12172,33 @@
       <c r="J312" t="s">
         <v>1122</v>
       </c>
+    </row>
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B313" t="s">
+        <v>384</v>
+      </c>
+      <c r="C313" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D313" t="s">
+        <v>404</v>
+      </c>
+      <c r="E313">
+        <v>1</v>
+      </c>
+      <c r="F313" t="s">
+        <v>1114</v>
+      </c>
+      <c r="G313" s="1" t="s">
+        <v>1160</v>
+      </c>
+      <c r="H313" t="s">
+        <v>57</v>
+      </c>
+      <c r="I313" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -12182,8 +12218,8 @@
     <hyperlink ref="G309" r:id="rId14" xr:uid="{2C0EEA17-F74E-4040-9F45-882756F31B0C}"/>
     <hyperlink ref="G310" r:id="rId15" xr:uid="{2B555168-39AE-48A2-BF30-BED6FA311D56}"/>
     <hyperlink ref="G311" r:id="rId16" xr:uid="{F81EECAB-5A10-48CF-B36A-05A56621D089}"/>
-    <hyperlink ref="G308" r:id="rId17" display="https://www.walmart.com/ip/9-in-1-Folding-Hex-Key-Set-Metric-Aluminum-Allen-Wrench-Multi-Purposes-Hex-Key-Tool-Non-Slip-for-Construction-Home-Decoration/723992410" xr:uid="{B077DD21-EE2C-4C9B-B6EF-22AF8FDEBBD5}"/>
-    <hyperlink ref="G202" r:id="rId18" xr:uid="{D9F4EE1D-73F1-477B-9CA8-D7387CE7A222}"/>
+    <hyperlink ref="G202" r:id="rId17" xr:uid="{D9F4EE1D-73F1-477B-9CA8-D7387CE7A222}"/>
+    <hyperlink ref="G313" r:id="rId18" xr:uid="{7351EFE1-3CF3-4E08-A5D4-DA6F0AA14EBB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>

</xml_diff>

<commit_message>
Changes coming to BOM
- Made some milestone changes. See below.
- Adjusted due date for 0.4.5 (pre-assembly testing).
  - Although the Micro Fit 3 profile is done, it's not tested.
  - The BOM needs to be broken out into the Sales BOM and the Manufacturing/Assembly BOM. This (kinda) exists with the Materials/Parts sections, but they are different things and need to be broken out.
- Documentation is progressing steadily in parallel, but can't progress while the BOM is changing (i.e. reference points might change).
</commit_message>
<xml_diff>
--- a/BOM/Unified Part List.xlsx
+++ b/BOM/Unified Part List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658FE920-CA2B-47A7-BC8E-81EC1DD6E29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8228C2C2-6B74-4448-AAFB-BB08053EC8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6EB0A7B6-C6D7-4759-8B58-841D5EFF92F5}"/>
+    <workbookView xWindow="2715" yWindow="3120" windowWidth="21495" windowHeight="12945" xr2:uid="{6EB0A7B6-C6D7-4759-8B58-841D5EFF92F5}"/>
   </bookViews>
   <sheets>
     <sheet name="source" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -3939,8 +3938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D318B5EB-87D8-4D97-AE82-574AF33D7DA4}">
   <dimension ref="A1:J313"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
-      <selection activeCell="J313" sqref="J313"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Prep for docs merge
Clearing out the /docs folder
</commit_message>
<xml_diff>
--- a/BOM/Unified Part List.xlsx
+++ b/BOM/Unified Part List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7D1B44-C867-477A-925C-BB6EA5E6D24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899DE07E-A2D8-468B-8D76-0964AA5ACE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2925" yWindow="615" windowWidth="21495" windowHeight="12945" xr2:uid="{6EB0A7B6-C6D7-4759-8B58-841D5EFF92F5}"/>
   </bookViews>
@@ -3974,8 +3974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D318B5EB-87D8-4D97-AE82-574AF33D7DA4}">
   <dimension ref="A1:J315"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="C171" sqref="C171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Widened latch open arc
</commit_message>
<xml_diff>
--- a/BOM/Unified Part List.xlsx
+++ b/BOM/Unified Part List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A844F24-391C-49C8-B962-E1E0ED363E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67D26CB-555F-454B-A580-8136571A84B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9375" yWindow="2175" windowWidth="17190" windowHeight="10350" xr2:uid="{6EB0A7B6-C6D7-4759-8B58-841D5EFF92F5}"/>
+    <workbookView xWindow="9375" yWindow="2175" windowWidth="17190" windowHeight="13665" xr2:uid="{6EB0A7B6-C6D7-4759-8B58-841D5EFF92F5}"/>
   </bookViews>
   <sheets>
     <sheet name="source" sheetId="1" r:id="rId1"/>
@@ -3994,7 +3994,7 @@
   <dimension ref="A1:J317"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C122" workbookViewId="0">
-      <selection activeCell="G132" sqref="G132"/>
+      <selection activeCell="C139" sqref="C139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Testing new X gantry and hotend
</commit_message>
<xml_diff>
--- a/BOM/Unified Part List.xlsx
+++ b/BOM/Unified Part List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0FD0F8-09A4-4CF8-87CA-268EF5A3050C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFF95AA-45C9-4A9A-AD24-A0A3B54A12CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3120" yWindow="2535" windowWidth="25455" windowHeight="13665" xr2:uid="{6EB0A7B6-C6D7-4759-8B58-841D5EFF92F5}"/>
+    <workbookView xWindow="-26415" yWindow="1125" windowWidth="25455" windowHeight="13665" xr2:uid="{6EB0A7B6-C6D7-4759-8B58-841D5EFF92F5}"/>
   </bookViews>
   <sheets>
     <sheet name="source" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="1187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2348" uniqueCount="1189">
   <si>
     <t>ID</t>
   </si>
@@ -3596,6 +3596,12 @@
   </si>
   <si>
     <t>Heater Cartridge, 20mm x 6mm</t>
+  </si>
+  <si>
+    <t>PN954</t>
+  </si>
+  <si>
+    <t>Fan, Radial, 40mm x 10mm, 12/24V</t>
   </si>
 </sst>
 </file>
@@ -3697,10 +3703,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}" name="Table13" displayName="Table13" ref="A1:J320" totalsRowShown="0">
-  <autoFilter ref="A1:J320" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J317">
-    <sortCondition ref="A1:A317"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}" name="Table13" displayName="Table13" ref="A1:J321" totalsRowShown="0">
+  <autoFilter ref="A1:J321" xr:uid="{BCCEB002-6247-475F-8E59-4D3290F5D0AB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J318">
+    <sortCondition ref="A1:A318"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{5013DA2C-AE55-4442-B536-8693A638A779}" name="ID"/>
@@ -4015,10 +4021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D318B5EB-87D8-4D97-AE82-574AF33D7DA4}">
-  <dimension ref="A1:J320"/>
+  <dimension ref="A1:J321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11346,13 +11352,13 @@
     </row>
     <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>310</v>
+        <v>1187</v>
       </c>
       <c r="B281" t="s">
         <v>247</v>
       </c>
       <c r="C281" t="s">
-        <v>311</v>
+        <v>1188</v>
       </c>
       <c r="D281" t="s">
         <v>400</v>
@@ -11360,23 +11366,18 @@
       <c r="F281" t="s">
         <v>6</v>
       </c>
-      <c r="G281" s="1" t="s">
-        <v>576</v>
-      </c>
-      <c r="H281" t="s">
-        <v>57</v>
-      </c>
+      <c r="G281" s="1"/>
       <c r="I281" s="5"/>
     </row>
     <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B282" t="s">
         <v>247</v>
       </c>
       <c r="C282" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D282" t="s">
         <v>400</v>
@@ -11385,7 +11386,7 @@
         <v>6</v>
       </c>
       <c r="G282" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H282" t="s">
         <v>57</v>
@@ -11394,13 +11395,13 @@
     </row>
     <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B283" t="s">
         <v>247</v>
       </c>
       <c r="C283" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D283" t="s">
         <v>400</v>
@@ -11409,25 +11410,22 @@
         <v>6</v>
       </c>
       <c r="G283" s="1" t="s">
-        <v>565</v>
+        <v>577</v>
       </c>
       <c r="H283" t="s">
         <v>57</v>
       </c>
       <c r="I283" s="5"/>
-      <c r="J283" t="s">
-        <v>316</v>
-      </c>
     </row>
     <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B284" t="s">
         <v>247</v>
       </c>
       <c r="C284" t="s">
-        <v>471</v>
+        <v>315</v>
       </c>
       <c r="D284" t="s">
         <v>400</v>
@@ -11436,110 +11434,110 @@
         <v>6</v>
       </c>
       <c r="G284" s="1" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="H284" t="s">
-        <v>318</v>
-      </c>
-      <c r="I284" s="5" t="s">
-        <v>319</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="I284" s="5"/>
       <c r="J284" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B285" t="s">
         <v>247</v>
       </c>
       <c r="C285" t="s">
-        <v>1050</v>
+        <v>471</v>
       </c>
       <c r="D285" t="s">
         <v>400</v>
       </c>
       <c r="F285" t="s">
-        <v>128</v>
+        <v>6</v>
       </c>
       <c r="G285" s="1" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="H285" t="s">
-        <v>32</v>
+        <v>318</v>
       </c>
       <c r="I285" s="5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="J285" t="s">
-        <v>683</v>
+        <v>320</v>
       </c>
     </row>
     <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B286" t="s">
         <v>247</v>
       </c>
       <c r="C286" t="s">
-        <v>435</v>
+        <v>1050</v>
       </c>
       <c r="D286" t="s">
         <v>400</v>
       </c>
       <c r="F286" t="s">
-        <v>6</v>
+        <v>128</v>
       </c>
       <c r="G286" s="1" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="H286" t="s">
-        <v>57</v>
-      </c>
-      <c r="I286" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="I286" s="5" t="s">
+        <v>322</v>
+      </c>
       <c r="J286" t="s">
-        <v>324</v>
+        <v>683</v>
       </c>
     </row>
     <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>464</v>
+        <v>323</v>
       </c>
       <c r="B287" t="s">
         <v>247</v>
       </c>
       <c r="C287" t="s">
-        <v>465</v>
+        <v>435</v>
       </c>
       <c r="D287" t="s">
         <v>400</v>
       </c>
-      <c r="E287">
-        <v>1</v>
-      </c>
-      <c r="F287" s="6" t="s">
+      <c r="F287" t="s">
         <v>6</v>
       </c>
       <c r="G287" s="1" t="s">
-        <v>682</v>
+        <v>562</v>
       </c>
       <c r="H287" t="s">
         <v>57</v>
       </c>
       <c r="I287" s="5"/>
+      <c r="J287" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>518</v>
+        <v>464</v>
       </c>
       <c r="B288" t="s">
         <v>247</v>
       </c>
       <c r="C288" t="s">
-        <v>519</v>
+        <v>465</v>
       </c>
       <c r="D288" t="s">
         <v>400</v>
@@ -11547,11 +11545,11 @@
       <c r="E288">
         <v>1</v>
       </c>
-      <c r="F288" t="s">
+      <c r="F288" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G288" s="1" t="s">
-        <v>561</v>
+        <v>682</v>
       </c>
       <c r="H288" t="s">
         <v>57</v>
@@ -11560,16 +11558,16 @@
     </row>
     <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B289" t="s">
         <v>247</v>
       </c>
       <c r="C289" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D289" t="s">
-        <v>455</v>
+        <v>400</v>
       </c>
       <c r="E289">
         <v>1</v>
@@ -11578,7 +11576,7 @@
         <v>6</v>
       </c>
       <c r="G289" s="1" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="H289" t="s">
         <v>57</v>
@@ -11587,40 +11585,40 @@
     </row>
     <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>325</v>
+        <v>520</v>
       </c>
       <c r="B290" t="s">
         <v>247</v>
       </c>
       <c r="C290" t="s">
-        <v>326</v>
+        <v>521</v>
       </c>
       <c r="D290" t="s">
-        <v>400</v>
+        <v>455</v>
+      </c>
+      <c r="E290">
+        <v>1</v>
       </c>
       <c r="F290" t="s">
         <v>6</v>
       </c>
       <c r="G290" s="1" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="H290" t="s">
         <v>57</v>
       </c>
       <c r="I290" s="5"/>
-      <c r="J290" t="s">
-        <v>327</v>
-      </c>
     </row>
     <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B291" t="s">
         <v>247</v>
       </c>
       <c r="C291" t="s">
-        <v>1185</v>
+        <v>326</v>
       </c>
       <c r="D291" t="s">
         <v>400</v>
@@ -11629,22 +11627,25 @@
         <v>6</v>
       </c>
       <c r="G291" s="1" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="H291" t="s">
         <v>57</v>
       </c>
       <c r="I291" s="5"/>
+      <c r="J291" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B292" t="s">
         <v>247</v>
       </c>
       <c r="C292" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="D292" t="s">
         <v>400</v>
@@ -11653,15 +11654,12 @@
         <v>6</v>
       </c>
       <c r="G292" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H292" t="s">
         <v>57</v>
       </c>
       <c r="I292" s="5"/>
-      <c r="J292" t="s">
-        <v>379</v>
-      </c>
     </row>
     <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
@@ -11671,7 +11669,7 @@
         <v>247</v>
       </c>
       <c r="C293" t="s">
-        <v>509</v>
+        <v>1186</v>
       </c>
       <c r="D293" t="s">
         <v>400</v>
@@ -11680,24 +11678,25 @@
         <v>6</v>
       </c>
       <c r="G293" s="1" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="H293" t="s">
-        <v>104</v>
-      </c>
-      <c r="I293" s="5" t="s">
-        <v>380</v>
+        <v>57</v>
+      </c>
+      <c r="I293" s="5"/>
+      <c r="J293" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B294" t="s">
         <v>247</v>
       </c>
       <c r="C294" t="s">
-        <v>391</v>
+        <v>509</v>
       </c>
       <c r="D294" t="s">
         <v>400</v>
@@ -11706,24 +11705,24 @@
         <v>6</v>
       </c>
       <c r="G294" s="1" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="H294" t="s">
-        <v>212</v>
+        <v>104</v>
       </c>
       <c r="I294" s="5" t="s">
-        <v>331</v>
+        <v>380</v>
       </c>
     </row>
     <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B295" t="s">
         <v>247</v>
       </c>
       <c r="C295" t="s">
-        <v>333</v>
+        <v>391</v>
       </c>
       <c r="D295" t="s">
         <v>400</v>
@@ -11732,24 +11731,24 @@
         <v>6</v>
       </c>
       <c r="G295" s="1" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="H295" t="s">
         <v>212</v>
       </c>
       <c r="I295" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B296" t="s">
         <v>247</v>
       </c>
       <c r="C296" t="s">
-        <v>1168</v>
+        <v>333</v>
       </c>
       <c r="D296" t="s">
         <v>400</v>
@@ -11758,76 +11757,76 @@
         <v>6</v>
       </c>
       <c r="G296" s="1" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="H296" t="s">
         <v>212</v>
       </c>
       <c r="I296" s="5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B297" t="s">
         <v>247</v>
       </c>
       <c r="C297" t="s">
-        <v>338</v>
+        <v>1168</v>
       </c>
       <c r="D297" t="s">
         <v>400</v>
       </c>
       <c r="F297" t="s">
-        <v>264</v>
+        <v>6</v>
       </c>
       <c r="G297" s="1" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="H297" t="s">
-        <v>339</v>
+        <v>212</v>
       </c>
       <c r="I297" s="5" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B298" t="s">
         <v>247</v>
       </c>
       <c r="C298" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D298" t="s">
         <v>400</v>
       </c>
       <c r="F298" t="s">
-        <v>6</v>
+        <v>264</v>
       </c>
       <c r="G298" s="1" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="H298" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="I298" s="5" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B299" t="s">
         <v>247</v>
       </c>
       <c r="C299" t="s">
-        <v>378</v>
+        <v>342</v>
       </c>
       <c r="D299" t="s">
         <v>400</v>
@@ -11836,24 +11835,24 @@
         <v>6</v>
       </c>
       <c r="G299" s="1" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="H299" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="I299" s="5" t="s">
-        <v>377</v>
+        <v>344</v>
       </c>
     </row>
     <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>478</v>
+        <v>345</v>
       </c>
       <c r="B300" t="s">
         <v>247</v>
       </c>
       <c r="C300" t="s">
-        <v>1051</v>
+        <v>378</v>
       </c>
       <c r="D300" t="s">
         <v>400</v>
@@ -11862,54 +11861,51 @@
         <v>6</v>
       </c>
       <c r="G300" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="H300" t="s">
-        <v>57</v>
-      </c>
-      <c r="I300" s="5"/>
-      <c r="J300" t="s">
-        <v>479</v>
+        <v>346</v>
+      </c>
+      <c r="I300" s="5" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>440</v>
+        <v>478</v>
       </c>
       <c r="B301" t="s">
-        <v>381</v>
+        <v>247</v>
       </c>
       <c r="C301" t="s">
-        <v>398</v>
+        <v>1051</v>
       </c>
       <c r="D301" t="s">
         <v>400</v>
-      </c>
-      <c r="E301">
-        <v>1</v>
       </c>
       <c r="F301" t="s">
         <v>6</v>
       </c>
       <c r="G301" s="1" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="H301" t="s">
-        <v>393</v>
-      </c>
-      <c r="I301" s="5">
-        <v>92003</v>
+        <v>57</v>
+      </c>
+      <c r="I301" s="5"/>
+      <c r="J301" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B302" t="s">
         <v>381</v>
       </c>
       <c r="C302" t="s">
-        <v>382</v>
+        <v>398</v>
       </c>
       <c r="D302" t="s">
         <v>400</v>
@@ -11918,58 +11914,60 @@
         <v>1</v>
       </c>
       <c r="F302" t="s">
-        <v>1108</v>
-      </c>
-      <c r="G302" t="s">
-        <v>1117</v>
+        <v>6</v>
+      </c>
+      <c r="G302" s="1" t="s">
+        <v>547</v>
       </c>
       <c r="H302" t="s">
-        <v>57</v>
-      </c>
-      <c r="I302" s="5"/>
-      <c r="J302" t="s">
-        <v>392</v>
+        <v>393</v>
+      </c>
+      <c r="I302" s="5">
+        <v>92003</v>
       </c>
     </row>
     <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B303" t="s">
         <v>381</v>
       </c>
       <c r="C303" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D303" t="s">
-        <v>455</v>
+        <v>400</v>
       </c>
       <c r="E303">
         <v>1</v>
       </c>
       <c r="F303" t="s">
-        <v>6</v>
+        <v>1108</v>
       </c>
       <c r="G303" t="s">
-        <v>669</v>
+        <v>1117</v>
       </c>
       <c r="H303" t="s">
         <v>57</v>
       </c>
       <c r="I303" s="5"/>
+      <c r="J303" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B304" t="s">
         <v>381</v>
       </c>
       <c r="C304" t="s">
-        <v>670</v>
+        <v>383</v>
       </c>
       <c r="D304" t="s">
-        <v>400</v>
+        <v>455</v>
       </c>
       <c r="E304">
         <v>1</v>
@@ -11977,8 +11975,8 @@
       <c r="F304" t="s">
         <v>6</v>
       </c>
-      <c r="G304" s="1" t="s">
-        <v>671</v>
+      <c r="G304" t="s">
+        <v>669</v>
       </c>
       <c r="H304" t="s">
         <v>57</v>
@@ -11987,13 +11985,13 @@
     </row>
     <row r="305" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B305" t="s">
         <v>381</v>
       </c>
       <c r="C305" t="s">
-        <v>384</v>
+        <v>670</v>
       </c>
       <c r="D305" t="s">
         <v>400</v>
@@ -12004,26 +12002,23 @@
       <c r="F305" t="s">
         <v>6</v>
       </c>
-      <c r="G305" t="s">
-        <v>1128</v>
+      <c r="G305" s="1" t="s">
+        <v>671</v>
       </c>
       <c r="H305" t="s">
         <v>57</v>
       </c>
       <c r="I305" s="5"/>
-      <c r="J305" t="s">
-        <v>425</v>
-      </c>
     </row>
     <row r="306" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B306" t="s">
         <v>381</v>
       </c>
       <c r="C306" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D306" t="s">
         <v>400</v>
@@ -12035,22 +12030,25 @@
         <v>6</v>
       </c>
       <c r="G306" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="H306" t="s">
         <v>57</v>
       </c>
       <c r="I306" s="5"/>
+      <c r="J306" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="307" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B307" t="s">
         <v>381</v>
       </c>
       <c r="C307" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D307" t="s">
         <v>400</v>
@@ -12062,25 +12060,22 @@
         <v>6</v>
       </c>
       <c r="G307" t="s">
-        <v>680</v>
+        <v>1127</v>
       </c>
       <c r="H307" t="s">
         <v>57</v>
       </c>
       <c r="I307" s="5"/>
-      <c r="J307" t="s">
-        <v>681</v>
-      </c>
     </row>
     <row r="308" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B308" t="s">
         <v>381</v>
       </c>
       <c r="C308" t="s">
-        <v>448</v>
+        <v>388</v>
       </c>
       <c r="D308" t="s">
         <v>400</v>
@@ -12092,22 +12087,25 @@
         <v>6</v>
       </c>
       <c r="G308" t="s">
-        <v>1105</v>
+        <v>680</v>
       </c>
       <c r="H308" t="s">
         <v>57</v>
       </c>
       <c r="I308" s="5"/>
+      <c r="J308" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="309" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B309" t="s">
         <v>381</v>
       </c>
       <c r="C309" t="s">
-        <v>679</v>
+        <v>448</v>
       </c>
       <c r="D309" t="s">
         <v>400</v>
@@ -12119,24 +12117,22 @@
         <v>6</v>
       </c>
       <c r="G309" t="s">
-        <v>676</v>
+        <v>1105</v>
       </c>
       <c r="H309" t="s">
-        <v>677</v>
-      </c>
-      <c r="I309" s="5" t="s">
-        <v>678</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="I309" s="5"/>
     </row>
     <row r="310" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B310" t="s">
         <v>381</v>
       </c>
       <c r="C310" t="s">
-        <v>386</v>
+        <v>679</v>
       </c>
       <c r="D310" t="s">
         <v>400</v>
@@ -12148,22 +12144,24 @@
         <v>6</v>
       </c>
       <c r="G310" t="s">
-        <v>1103</v>
+        <v>676</v>
       </c>
       <c r="H310" t="s">
-        <v>1104</v>
-      </c>
-      <c r="I310" s="5"/>
+        <v>677</v>
+      </c>
+      <c r="I310" s="5" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="311" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B311" t="s">
         <v>381</v>
       </c>
       <c r="C311" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D311" t="s">
         <v>400</v>
@@ -12175,24 +12173,22 @@
         <v>6</v>
       </c>
       <c r="G311" t="s">
-        <v>672</v>
+        <v>1103</v>
       </c>
       <c r="H311" t="s">
-        <v>673</v>
-      </c>
-      <c r="I311" s="5" t="s">
-        <v>674</v>
-      </c>
+        <v>1104</v>
+      </c>
+      <c r="I311" s="5"/>
     </row>
     <row r="312" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B312" t="s">
         <v>381</v>
       </c>
       <c r="C312" t="s">
-        <v>1057</v>
+        <v>387</v>
       </c>
       <c r="D312" t="s">
         <v>400</v>
@@ -12203,28 +12199,25 @@
       <c r="F312" t="s">
         <v>6</v>
       </c>
-      <c r="G312" s="1" t="s">
-        <v>1100</v>
+      <c r="G312" t="s">
+        <v>672</v>
       </c>
       <c r="H312" t="s">
-        <v>1101</v>
+        <v>673</v>
       </c>
       <c r="I312" s="5" t="s">
-        <v>1102</v>
-      </c>
-      <c r="J312" t="s">
-        <v>666</v>
+        <v>674</v>
       </c>
     </row>
     <row r="313" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>1161</v>
+        <v>452</v>
       </c>
       <c r="B313" t="s">
         <v>381</v>
       </c>
       <c r="C313" t="s">
-        <v>1155</v>
+        <v>1057</v>
       </c>
       <c r="D313" t="s">
         <v>400</v>
@@ -12233,92 +12226,97 @@
         <v>1</v>
       </c>
       <c r="F313" t="s">
-        <v>1156</v>
+        <v>6</v>
       </c>
       <c r="G313" s="1" t="s">
-        <v>1157</v>
+        <v>1100</v>
       </c>
       <c r="H313" t="s">
-        <v>1158</v>
+        <v>1101</v>
       </c>
       <c r="I313" s="5" t="s">
-        <v>1159</v>
+        <v>1102</v>
       </c>
       <c r="J313" t="s">
-        <v>1160</v>
+        <v>666</v>
       </c>
     </row>
     <row r="314" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>461</v>
+        <v>1161</v>
       </c>
       <c r="B314" t="s">
         <v>381</v>
       </c>
       <c r="C314" t="s">
-        <v>667</v>
+        <v>1155</v>
       </c>
       <c r="D314" t="s">
         <v>400</v>
       </c>
       <c r="E314">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F314" t="s">
-        <v>6</v>
-      </c>
-      <c r="G314" t="s">
-        <v>668</v>
+        <v>1156</v>
+      </c>
+      <c r="G314" s="1" t="s">
+        <v>1157</v>
       </c>
       <c r="H314" t="s">
-        <v>462</v>
+        <v>1158</v>
       </c>
       <c r="I314" s="5" t="s">
-        <v>463</v>
+        <v>1159</v>
       </c>
       <c r="J314" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="315" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>453</v>
+        <v>461</v>
       </c>
       <c r="B315" t="s">
         <v>381</v>
       </c>
       <c r="C315" t="s">
-        <v>390</v>
+        <v>667</v>
       </c>
       <c r="D315" t="s">
-        <v>455</v>
+        <v>400</v>
       </c>
       <c r="E315">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F315" t="s">
-        <v>1108</v>
+        <v>6</v>
       </c>
       <c r="G315" t="s">
-        <v>1151</v>
+        <v>668</v>
       </c>
       <c r="H315" t="s">
-        <v>57</v>
-      </c>
-      <c r="I315" s="5"/>
+        <v>462</v>
+      </c>
+      <c r="I315" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="J315" t="s">
+        <v>1162</v>
+      </c>
     </row>
     <row r="316" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>515</v>
+        <v>453</v>
       </c>
       <c r="B316" t="s">
         <v>381</v>
       </c>
       <c r="C316" t="s">
-        <v>516</v>
+        <v>390</v>
       </c>
       <c r="D316" t="s">
-        <v>400</v>
+        <v>455</v>
       </c>
       <c r="E316">
         <v>1</v>
@@ -12326,31 +12324,26 @@
       <c r="F316" t="s">
         <v>1108</v>
       </c>
-      <c r="G316" s="1" t="s">
-        <v>1107</v>
+      <c r="G316" t="s">
+        <v>1151</v>
       </c>
       <c r="H316" t="s">
-        <v>1106</v>
-      </c>
-      <c r="I316" s="5" t="s">
-        <v>1109</v>
-      </c>
-      <c r="J316" t="s">
-        <v>727</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="I316" s="5"/>
     </row>
     <row r="317" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B317" t="s">
         <v>381</v>
       </c>
       <c r="C317" t="s">
-        <v>1115</v>
+        <v>516</v>
       </c>
       <c r="D317" t="s">
-        <v>455</v>
+        <v>400</v>
       </c>
       <c r="E317">
         <v>1</v>
@@ -12359,25 +12352,27 @@
         <v>1108</v>
       </c>
       <c r="G317" s="1" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="H317" t="s">
-        <v>57</v>
-      </c>
-      <c r="I317" s="5"/>
+        <v>1106</v>
+      </c>
+      <c r="I317" s="5" t="s">
+        <v>1109</v>
+      </c>
       <c r="J317" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="318" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>1112</v>
+        <v>517</v>
       </c>
       <c r="B318" t="s">
         <v>381</v>
       </c>
       <c r="C318" t="s">
-        <v>1113</v>
+        <v>1115</v>
       </c>
       <c r="D318" t="s">
         <v>455</v>
@@ -12389,7 +12384,7 @@
         <v>1108</v>
       </c>
       <c r="G318" s="1" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
       <c r="H318" t="s">
         <v>57</v>
@@ -12401,43 +12396,43 @@
     </row>
     <row r="319" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="B319" t="s">
         <v>381</v>
       </c>
       <c r="C319" t="s">
-        <v>1083</v>
+        <v>1113</v>
       </c>
       <c r="D319" t="s">
-        <v>400</v>
+        <v>455</v>
       </c>
       <c r="E319">
         <v>1</v>
       </c>
       <c r="F319" t="s">
-        <v>6</v>
-      </c>
-      <c r="G319" t="s">
-        <v>1129</v>
+        <v>1108</v>
+      </c>
+      <c r="G319" s="1" t="s">
+        <v>1114</v>
       </c>
       <c r="H319" t="s">
         <v>57</v>
       </c>
       <c r="I319" s="5"/>
       <c r="J319" t="s">
-        <v>1116</v>
+        <v>726</v>
       </c>
     </row>
     <row r="320" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>1152</v>
+        <v>1111</v>
       </c>
       <c r="B320" t="s">
         <v>381</v>
       </c>
       <c r="C320" t="s">
-        <v>1153</v>
+        <v>1083</v>
       </c>
       <c r="D320" t="s">
         <v>400</v>
@@ -12446,22 +12441,52 @@
         <v>1</v>
       </c>
       <c r="F320" t="s">
-        <v>1108</v>
-      </c>
-      <c r="G320" s="1" t="s">
-        <v>1154</v>
+        <v>6</v>
+      </c>
+      <c r="G320" t="s">
+        <v>1129</v>
       </c>
       <c r="H320" t="s">
         <v>57</v>
       </c>
       <c r="I320" s="5"/>
+      <c r="J320" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B321" t="s">
+        <v>381</v>
+      </c>
+      <c r="C321" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D321" t="s">
+        <v>400</v>
+      </c>
+      <c r="E321">
+        <v>1</v>
+      </c>
+      <c r="F321" t="s">
+        <v>1108</v>
+      </c>
+      <c r="G321" s="1" t="s">
+        <v>1154</v>
+      </c>
+      <c r="H321" t="s">
+        <v>57</v>
+      </c>
+      <c r="I321" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G146" r:id="rId1" xr:uid="{EC7FA136-5E31-4921-B95C-7A464909BD66}"/>
     <hyperlink ref="G148" r:id="rId2" xr:uid="{71E787F6-211B-4241-8E76-CF22B248E3DB}"/>
     <hyperlink ref="G149" r:id="rId3" xr:uid="{3B791CF3-5818-4AE7-9B9F-37B6ECA27E60}"/>
-    <hyperlink ref="G304" r:id="rId4" xr:uid="{D022707A-EC6F-4C5C-81E7-41B5B3AD1C37}"/>
+    <hyperlink ref="G305" r:id="rId4" xr:uid="{D022707A-EC6F-4C5C-81E7-41B5B3AD1C37}"/>
     <hyperlink ref="G175" r:id="rId5" xr:uid="{6EB12907-0812-466A-9C43-4E735EACE634}"/>
     <hyperlink ref="G22" r:id="rId6" xr:uid="{A8AB8D34-CB3C-46EE-A784-757B50AE5104}"/>
     <hyperlink ref="G26" r:id="rId7" xr:uid="{83EFA558-6064-4A22-B4F0-E0BF43E7DD16}"/>
@@ -12470,12 +12495,12 @@
     <hyperlink ref="G164" r:id="rId10" xr:uid="{ED98147D-02B0-46E8-A6F9-B76FDE7131EE}"/>
     <hyperlink ref="G166" r:id="rId11" xr:uid="{56373C9C-C396-41A5-BBF0-2B2826F6857D}"/>
     <hyperlink ref="G167" r:id="rId12" xr:uid="{3BB5FDD4-07DA-4F8C-A384-18F64B935003}"/>
-    <hyperlink ref="G312" r:id="rId13" xr:uid="{D66D6780-581B-46DF-ADF0-5A25F6EAFD70}"/>
-    <hyperlink ref="G316" r:id="rId14" xr:uid="{2C0EEA17-F74E-4040-9F45-882756F31B0C}"/>
-    <hyperlink ref="G317" r:id="rId15" xr:uid="{2B555168-39AE-48A2-BF30-BED6FA311D56}"/>
-    <hyperlink ref="G318" r:id="rId16" xr:uid="{F81EECAB-5A10-48CF-B36A-05A56621D089}"/>
+    <hyperlink ref="G313" r:id="rId13" xr:uid="{D66D6780-581B-46DF-ADF0-5A25F6EAFD70}"/>
+    <hyperlink ref="G317" r:id="rId14" xr:uid="{2C0EEA17-F74E-4040-9F45-882756F31B0C}"/>
+    <hyperlink ref="G318" r:id="rId15" xr:uid="{2B555168-39AE-48A2-BF30-BED6FA311D56}"/>
+    <hyperlink ref="G319" r:id="rId16" xr:uid="{F81EECAB-5A10-48CF-B36A-05A56621D089}"/>
     <hyperlink ref="G208" r:id="rId17" xr:uid="{D9F4EE1D-73F1-477B-9CA8-D7387CE7A222}"/>
-    <hyperlink ref="G320" r:id="rId18" xr:uid="{7351EFE1-3CF3-4E08-A5D4-DA6F0AA14EBB}"/>
+    <hyperlink ref="G321" r:id="rId18" xr:uid="{7351EFE1-3CF3-4E08-A5D4-DA6F0AA14EBB}"/>
     <hyperlink ref="G4" r:id="rId19" xr:uid="{D4BAD1AB-86AD-4189-AE9D-076737468EDD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>